<commit_message>
adiccion de las correciones de DM HLS
</commit_message>
<xml_diff>
--- a/codigo_final_organizado/Aplicaciones/Aplicaciones_puras/Resultados_Electricity_Final/electricity_serie_0_resultados_full.xlsx
+++ b/codigo_final_organizado/Aplicaciones/Aplicaciones_puras/Resultados_Electricity_Final/electricity_serie_0_resultados_full.xlsx
@@ -523,7 +523,7 @@
         <v>2.925520793545424</v>
       </c>
       <c r="K2" t="n">
-        <v>3.480522011333322</v>
+        <v>3.378118867953183</v>
       </c>
     </row>
     <row r="3">
@@ -558,7 +558,7 @@
         <v>2.594210902604413</v>
       </c>
       <c r="K3" t="n">
-        <v>3.442207765867133</v>
+        <v>3.130778146408153</v>
       </c>
     </row>
     <row r="4">
@@ -593,7 +593,7 @@
         <v>1.960757881245542</v>
       </c>
       <c r="K4" t="n">
-        <v>3.832141090971911</v>
+        <v>3.584090938229371</v>
       </c>
     </row>
     <row r="5">
@@ -628,7 +628,7 @@
         <v>1.525057750975637</v>
       </c>
       <c r="K5" t="n">
-        <v>3.886349562396942</v>
+        <v>3.63921249041532</v>
       </c>
     </row>
     <row r="6">
@@ -663,7 +663,7 @@
         <v>1.52716259180392</v>
       </c>
       <c r="K6" t="n">
-        <v>3.872460828709164</v>
+        <v>3.609880350062108</v>
       </c>
     </row>
     <row r="7">
@@ -698,7 +698,7 @@
         <v>2.089103999035299</v>
       </c>
       <c r="K7" t="n">
-        <v>3.971852624363529</v>
+        <v>3.705518894271908</v>
       </c>
     </row>
     <row r="8">
@@ -733,7 +733,7 @@
         <v>1.732208502183915</v>
       </c>
       <c r="K8" t="n">
-        <v>3.980691499321711</v>
+        <v>3.730152199424272</v>
       </c>
     </row>
     <row r="9">
@@ -768,7 +768,7 @@
         <v>1.781945169349529</v>
       </c>
       <c r="K9" t="n">
-        <v>3.929899008117093</v>
+        <v>3.666130060929392</v>
       </c>
     </row>
     <row r="10">
@@ -803,7 +803,7 @@
         <v>1.643567142013495</v>
       </c>
       <c r="K10" t="n">
-        <v>3.928024218634905</v>
+        <v>3.667144009078122</v>
       </c>
     </row>
     <row r="11">
@@ -838,7 +838,7 @@
         <v>1.844681550063179</v>
       </c>
       <c r="K11" t="n">
-        <v>4.0028608077117</v>
+        <v>3.738117578702732</v>
       </c>
     </row>
     <row r="12">
@@ -873,7 +873,7 @@
         <v>1.715717939514911</v>
       </c>
       <c r="K12" t="n">
-        <v>3.896788953222869</v>
+        <v>3.683428767109539</v>
       </c>
     </row>
     <row r="13">
@@ -908,7 +908,7 @@
         <v>1.33706758191068</v>
       </c>
       <c r="K13" t="n">
-        <v>3.619358345788773</v>
+        <v>3.378243987824212</v>
       </c>
     </row>
     <row r="14">
@@ -943,7 +943,7 @@
         <v>5.637124946295703</v>
       </c>
       <c r="K14" t="n">
-        <v>5.064577792196883</v>
+        <v>4.519516751660177</v>
       </c>
     </row>
     <row r="15">
@@ -978,7 +978,7 @@
         <v>13.74946082406465</v>
       </c>
       <c r="K15" t="n">
-        <v>15.64509776757349</v>
+        <v>13.92376511200364</v>
       </c>
     </row>
     <row r="16">
@@ -1013,7 +1013,7 @@
         <v>9.895269065787287</v>
       </c>
       <c r="K16" t="n">
-        <v>8.192832615420228</v>
+        <v>9.685203277971254</v>
       </c>
     </row>
     <row r="17">
@@ -1048,7 +1048,7 @@
         <v>1.6057583227182</v>
       </c>
       <c r="K17" t="n">
-        <v>4.127955298280461</v>
+        <v>3.942145086725423</v>
       </c>
     </row>
     <row r="18">
@@ -1083,7 +1083,7 @@
         <v>2.45521316539933</v>
       </c>
       <c r="K18" t="n">
-        <v>3.610580868546021</v>
+        <v>3.40172745782657</v>
       </c>
     </row>
     <row r="19">
@@ -1118,7 +1118,7 @@
         <v>3.211364490559203</v>
       </c>
       <c r="K19" t="n">
-        <v>3.604950993415729</v>
+        <v>3.565318386833658</v>
       </c>
     </row>
     <row r="20">
@@ -1153,7 +1153,7 @@
         <v>2.660586763748931</v>
       </c>
       <c r="K20" t="n">
-        <v>3.21006181197327</v>
+        <v>3.089110762771786</v>
       </c>
     </row>
     <row r="21">
@@ -1188,7 +1188,7 @@
         <v>2.183669486298967</v>
       </c>
       <c r="K21" t="n">
-        <v>2.919484537864573</v>
+        <v>2.695026445706866</v>
       </c>
     </row>
     <row r="22">
@@ -1223,7 +1223,7 @@
         <v>1.374940234592161</v>
       </c>
       <c r="K22" t="n">
-        <v>3.230936480038492</v>
+        <v>2.95751578239483</v>
       </c>
     </row>
     <row r="23">
@@ -1258,7 +1258,7 @@
         <v>2.029910122480708</v>
       </c>
       <c r="K23" t="n">
-        <v>3.380976227292801</v>
+        <v>3.170131192362806</v>
       </c>
     </row>
     <row r="24">
@@ -1293,7 +1293,7 @@
         <v>2.448133529151313</v>
       </c>
       <c r="K24" t="n">
-        <v>3.474744463472571</v>
+        <v>3.179276765730073</v>
       </c>
     </row>
     <row r="25">
@@ -1328,7 +1328,7 @@
         <v>1.442606730237687</v>
       </c>
       <c r="K25" t="n">
-        <v>3.573628527144211</v>
+        <v>3.333213506255694</v>
       </c>
     </row>
   </sheetData>
@@ -11868,7 +11868,7 @@
         <v>0.16</v>
       </c>
       <c r="C809" t="n">
-        <v>0</v>
+        <v>0.04166666666666666</v>
       </c>
     </row>
     <row r="810">
@@ -11881,7 +11881,7 @@
         <v>0.17</v>
       </c>
       <c r="C810" t="n">
-        <v>0</v>
+        <v>0.04166666666666666</v>
       </c>
     </row>
     <row r="811">
@@ -11894,7 +11894,7 @@
         <v>0.18</v>
       </c>
       <c r="C811" t="n">
-        <v>0</v>
+        <v>0.04166666666666666</v>
       </c>
     </row>
     <row r="812">
@@ -11907,7 +11907,7 @@
         <v>0.19</v>
       </c>
       <c r="C812" t="n">
-        <v>0</v>
+        <v>0.04166666666666666</v>
       </c>
     </row>
     <row r="813">
@@ -11920,7 +11920,7 @@
         <v>0.2</v>
       </c>
       <c r="C813" t="n">
-        <v>0</v>
+        <v>0.04166666666666666</v>
       </c>
     </row>
     <row r="814">
@@ -11933,7 +11933,7 @@
         <v>0.21</v>
       </c>
       <c r="C814" t="n">
-        <v>0</v>
+        <v>0.04166666666666666</v>
       </c>
     </row>
     <row r="815">
@@ -11946,7 +11946,7 @@
         <v>0.22</v>
       </c>
       <c r="C815" t="n">
-        <v>0</v>
+        <v>0.04166666666666666</v>
       </c>
     </row>
     <row r="816">
@@ -12141,7 +12141,7 @@
         <v>0.37</v>
       </c>
       <c r="C830" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.08333333333333333</v>
       </c>
     </row>
     <row r="831">
@@ -12154,7 +12154,7 @@
         <v>0.38</v>
       </c>
       <c r="C831" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.08333333333333333</v>
       </c>
     </row>
     <row r="832">
@@ -12167,7 +12167,7 @@
         <v>0.39</v>
       </c>
       <c r="C832" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.08333333333333333</v>
       </c>
     </row>
     <row r="833">
@@ -12180,7 +12180,7 @@
         <v>0.4</v>
       </c>
       <c r="C833" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="834">
@@ -12193,7 +12193,7 @@
         <v>0.41</v>
       </c>
       <c r="C834" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="835">
@@ -12206,7 +12206,7 @@
         <v>0.42</v>
       </c>
       <c r="C835" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="836">
@@ -12219,7 +12219,7 @@
         <v>0.43</v>
       </c>
       <c r="C836" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.2083333333333333</v>
       </c>
     </row>
     <row r="837">
@@ -12232,7 +12232,7 @@
         <v>0.44</v>
       </c>
       <c r="C837" t="n">
-        <v>0.125</v>
+        <v>0.2083333333333333</v>
       </c>
     </row>
     <row r="838">
@@ -12245,7 +12245,7 @@
         <v>0.45</v>
       </c>
       <c r="C838" t="n">
-        <v>0.125</v>
+        <v>0.2083333333333333</v>
       </c>
     </row>
     <row r="839">
@@ -12258,7 +12258,7 @@
         <v>0.46</v>
       </c>
       <c r="C839" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="840">
@@ -12271,7 +12271,7 @@
         <v>0.47</v>
       </c>
       <c r="C840" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="841">
@@ -12284,7 +12284,7 @@
         <v>0.48</v>
       </c>
       <c r="C841" t="n">
-        <v>0.2083333333333333</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="842">
@@ -12297,7 +12297,7 @@
         <v>0.49</v>
       </c>
       <c r="C842" t="n">
-        <v>0.25</v>
+        <v>0.2916666666666667</v>
       </c>
     </row>
     <row r="843">
@@ -12310,7 +12310,7 @@
         <v>0.5</v>
       </c>
       <c r="C843" t="n">
-        <v>0.2916666666666667</v>
+        <v>0.4166666666666667</v>
       </c>
     </row>
     <row r="844">
@@ -12336,7 +12336,7 @@
         <v>0.52</v>
       </c>
       <c r="C845" t="n">
-        <v>0.4166666666666667</v>
+        <v>0.4583333333333333</v>
       </c>
     </row>
     <row r="846">
@@ -12375,7 +12375,7 @@
         <v>0.55</v>
       </c>
       <c r="C848" t="n">
-        <v>0.7916666666666666</v>
+        <v>0.8333333333333334</v>
       </c>
     </row>
     <row r="849">
@@ -12388,7 +12388,7 @@
         <v>0.5600000000000001</v>
       </c>
       <c r="C849" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.9166666666666666</v>
       </c>
     </row>
     <row r="850">
@@ -12544,7 +12544,7 @@
         <v>0.68</v>
       </c>
       <c r="C861" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.9583333333333334</v>
       </c>
     </row>
     <row r="862">
@@ -12557,7 +12557,7 @@
         <v>0.6900000000000001</v>
       </c>
       <c r="C862" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.9583333333333334</v>
       </c>
     </row>
     <row r="863">
@@ -12570,7 +12570,7 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="C863" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.9583333333333334</v>
       </c>
     </row>
     <row r="864">
@@ -12583,7 +12583,7 @@
         <v>0.7100000000000001</v>
       </c>
       <c r="C864" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.9583333333333334</v>
       </c>
     </row>
     <row r="865">
@@ -12596,7 +12596,7 @@
         <v>0.72</v>
       </c>
       <c r="C865" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.9583333333333334</v>
       </c>
     </row>
     <row r="866">

</xml_diff>

<commit_message>
Correcion a Diebold Mariano y revision de Cap1
</commit_message>
<xml_diff>
--- a/codigo_final_organizado/Aplicaciones/Aplicaciones_puras/Resultados_Electricity_Final/electricity_serie_0_resultados_full.xlsx
+++ b/codigo_final_organizado/Aplicaciones/Aplicaciones_puras/Resultados_Electricity_Final/electricity_serie_0_resultados_full.xlsx
@@ -523,7 +523,7 @@
         <v>2.925520793545424</v>
       </c>
       <c r="K2" t="n">
-        <v>3.378118867953183</v>
+        <v>3.758027037470606</v>
       </c>
     </row>
     <row r="3">
@@ -558,7 +558,7 @@
         <v>2.594210902604413</v>
       </c>
       <c r="K3" t="n">
-        <v>3.130778146408153</v>
+        <v>3.423949234137423</v>
       </c>
     </row>
     <row r="4">
@@ -593,7 +593,7 @@
         <v>1.960757881245542</v>
       </c>
       <c r="K4" t="n">
-        <v>3.584090938229371</v>
+        <v>3.749313837658861</v>
       </c>
     </row>
     <row r="5">
@@ -628,7 +628,7 @@
         <v>1.525057750975637</v>
       </c>
       <c r="K5" t="n">
-        <v>3.63921249041532</v>
+        <v>3.79187289159037</v>
       </c>
     </row>
     <row r="6">
@@ -663,7 +663,7 @@
         <v>1.52716259180392</v>
       </c>
       <c r="K6" t="n">
-        <v>3.609880350062108</v>
+        <v>3.796472818008077</v>
       </c>
     </row>
     <row r="7">
@@ -698,7 +698,7 @@
         <v>2.089103999035299</v>
       </c>
       <c r="K7" t="n">
-        <v>3.705518894271908</v>
+        <v>3.88462698097165</v>
       </c>
     </row>
     <row r="8">
@@ -733,7 +733,7 @@
         <v>1.732208502183915</v>
       </c>
       <c r="K8" t="n">
-        <v>3.730152199424272</v>
+        <v>3.875022854871307</v>
       </c>
     </row>
     <row r="9">
@@ -768,7 +768,7 @@
         <v>1.781945169349529</v>
       </c>
       <c r="K9" t="n">
-        <v>3.666130060929392</v>
+        <v>3.842861328867081</v>
       </c>
     </row>
     <row r="10">
@@ -803,7 +803,7 @@
         <v>1.643567142013495</v>
       </c>
       <c r="K10" t="n">
-        <v>3.667144009078122</v>
+        <v>3.838283094437498</v>
       </c>
     </row>
     <row r="11">
@@ -838,7 +838,7 @@
         <v>1.844681550063179</v>
       </c>
       <c r="K11" t="n">
-        <v>3.738117578702732</v>
+        <v>3.907072762435249</v>
       </c>
     </row>
     <row r="12">
@@ -873,7 +873,7 @@
         <v>1.715717939514911</v>
       </c>
       <c r="K12" t="n">
-        <v>3.683428767109539</v>
+        <v>3.865202952844662</v>
       </c>
     </row>
     <row r="13">
@@ -908,7 +908,7 @@
         <v>1.33706758191068</v>
       </c>
       <c r="K13" t="n">
-        <v>3.378243987824212</v>
+        <v>3.621952348279919</v>
       </c>
     </row>
     <row r="14">
@@ -943,7 +943,7 @@
         <v>5.637124946295703</v>
       </c>
       <c r="K14" t="n">
-        <v>4.519516751660177</v>
+        <v>4.364350586382203</v>
       </c>
     </row>
     <row r="15">
@@ -978,7 +978,7 @@
         <v>13.74946082406465</v>
       </c>
       <c r="K15" t="n">
-        <v>13.92376511200364</v>
+        <v>11.18854862243428</v>
       </c>
     </row>
     <row r="16">
@@ -1013,7 +1013,7 @@
         <v>9.895269065787287</v>
       </c>
       <c r="K16" t="n">
-        <v>9.685203277971254</v>
+        <v>12.93301175572414</v>
       </c>
     </row>
     <row r="17">
@@ -1048,7 +1048,7 @@
         <v>1.6057583227182</v>
       </c>
       <c r="K17" t="n">
-        <v>3.942145086725423</v>
+        <v>4.230612849622545</v>
       </c>
     </row>
     <row r="18">
@@ -1083,7 +1083,7 @@
         <v>2.45521316539933</v>
       </c>
       <c r="K18" t="n">
-        <v>3.40172745782657</v>
+        <v>3.593957573726737</v>
       </c>
     </row>
     <row r="19">
@@ -1118,7 +1118,7 @@
         <v>3.211364490559203</v>
       </c>
       <c r="K19" t="n">
-        <v>3.565318386833658</v>
+        <v>3.889728855548245</v>
       </c>
     </row>
     <row r="20">
@@ -1153,7 +1153,7 @@
         <v>2.660586763748931</v>
       </c>
       <c r="K20" t="n">
-        <v>3.089110762771786</v>
+        <v>3.403864253255919</v>
       </c>
     </row>
     <row r="21">
@@ -1188,7 +1188,7 @@
         <v>2.183669486298967</v>
       </c>
       <c r="K21" t="n">
-        <v>2.695026445706866</v>
+        <v>2.96815869810564</v>
       </c>
     </row>
     <row r="22">
@@ -1223,7 +1223,7 @@
         <v>1.374940234592161</v>
       </c>
       <c r="K22" t="n">
-        <v>2.95751578239483</v>
+        <v>3.198703415617933</v>
       </c>
     </row>
     <row r="23">
@@ -1258,7 +1258,7 @@
         <v>2.029910122480708</v>
       </c>
       <c r="K23" t="n">
-        <v>3.170131192362806</v>
+        <v>3.407760641777841</v>
       </c>
     </row>
     <row r="24">
@@ -1293,7 +1293,7 @@
         <v>2.448133529151313</v>
       </c>
       <c r="K24" t="n">
-        <v>3.179276765730073</v>
+        <v>3.456431200976954</v>
       </c>
     </row>
     <row r="25">
@@ -1328,7 +1328,7 @@
         <v>1.442606730237687</v>
       </c>
       <c r="K25" t="n">
-        <v>3.333213506255694</v>
+        <v>3.557904840160039</v>
       </c>
     </row>
   </sheetData>
@@ -11738,7 +11738,7 @@
         <v>0.06</v>
       </c>
       <c r="C799" t="n">
-        <v>0</v>
+        <v>0.04166666666666666</v>
       </c>
     </row>
     <row r="800">
@@ -11751,7 +11751,7 @@
         <v>0.06999999999999999</v>
       </c>
       <c r="C800" t="n">
-        <v>0</v>
+        <v>0.04166666666666666</v>
       </c>
     </row>
     <row r="801">
@@ -11764,7 +11764,7 @@
         <v>0.08</v>
       </c>
       <c r="C801" t="n">
-        <v>0</v>
+        <v>0.04166666666666666</v>
       </c>
     </row>
     <row r="802">
@@ -11777,7 +11777,7 @@
         <v>0.09</v>
       </c>
       <c r="C802" t="n">
-        <v>0</v>
+        <v>0.04166666666666666</v>
       </c>
     </row>
     <row r="803">
@@ -11790,7 +11790,7 @@
         <v>0.09999999999999999</v>
       </c>
       <c r="C803" t="n">
-        <v>0</v>
+        <v>0.04166666666666666</v>
       </c>
     </row>
     <row r="804">
@@ -11803,7 +11803,7 @@
         <v>0.11</v>
       </c>
       <c r="C804" t="n">
-        <v>0</v>
+        <v>0.04166666666666666</v>
       </c>
     </row>
     <row r="805">
@@ -11816,7 +11816,7 @@
         <v>0.12</v>
       </c>
       <c r="C805" t="n">
-        <v>0</v>
+        <v>0.04166666666666666</v>
       </c>
     </row>
     <row r="806">
@@ -11829,7 +11829,7 @@
         <v>0.13</v>
       </c>
       <c r="C806" t="n">
-        <v>0</v>
+        <v>0.04166666666666666</v>
       </c>
     </row>
     <row r="807">
@@ -11842,7 +11842,7 @@
         <v>0.14</v>
       </c>
       <c r="C807" t="n">
-        <v>0</v>
+        <v>0.04166666666666666</v>
       </c>
     </row>
     <row r="808">
@@ -11855,7 +11855,7 @@
         <v>0.15</v>
       </c>
       <c r="C808" t="n">
-        <v>0</v>
+        <v>0.04166666666666666</v>
       </c>
     </row>
     <row r="809">
@@ -12063,7 +12063,7 @@
         <v>0.31</v>
       </c>
       <c r="C824" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.08333333333333333</v>
       </c>
     </row>
     <row r="825">
@@ -12076,7 +12076,7 @@
         <v>0.32</v>
       </c>
       <c r="C825" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.08333333333333333</v>
       </c>
     </row>
     <row r="826">
@@ -12089,7 +12089,7 @@
         <v>0.33</v>
       </c>
       <c r="C826" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.08333333333333333</v>
       </c>
     </row>
     <row r="827">
@@ -12102,7 +12102,7 @@
         <v>0.34</v>
       </c>
       <c r="C827" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.08333333333333333</v>
       </c>
     </row>
     <row r="828">
@@ -12115,7 +12115,7 @@
         <v>0.35</v>
       </c>
       <c r="C828" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.08333333333333333</v>
       </c>
     </row>
     <row r="829">
@@ -12128,7 +12128,7 @@
         <v>0.36</v>
       </c>
       <c r="C829" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="830">
@@ -12141,7 +12141,7 @@
         <v>0.37</v>
       </c>
       <c r="C830" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="831">
@@ -12154,7 +12154,7 @@
         <v>0.38</v>
       </c>
       <c r="C831" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="832">
@@ -12167,7 +12167,7 @@
         <v>0.39</v>
       </c>
       <c r="C832" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.2083333333333333</v>
       </c>
     </row>
     <row r="833">
@@ -12180,7 +12180,7 @@
         <v>0.4</v>
       </c>
       <c r="C833" t="n">
-        <v>0.125</v>
+        <v>0.2083333333333333</v>
       </c>
     </row>
     <row r="834">
@@ -12193,7 +12193,7 @@
         <v>0.41</v>
       </c>
       <c r="C834" t="n">
-        <v>0.125</v>
+        <v>0.2083333333333333</v>
       </c>
     </row>
     <row r="835">
@@ -12206,7 +12206,7 @@
         <v>0.42</v>
       </c>
       <c r="C835" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.2083333333333333</v>
       </c>
     </row>
     <row r="836">
@@ -12284,7 +12284,7 @@
         <v>0.48</v>
       </c>
       <c r="C841" t="n">
-        <v>0.25</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="842">
@@ -12297,7 +12297,7 @@
         <v>0.49</v>
       </c>
       <c r="C842" t="n">
-        <v>0.2916666666666667</v>
+        <v>0.4166666666666667</v>
       </c>
     </row>
     <row r="843">
@@ -12310,7 +12310,7 @@
         <v>0.5</v>
       </c>
       <c r="C843" t="n">
-        <v>0.4166666666666667</v>
+        <v>0.4583333333333333</v>
       </c>
     </row>
     <row r="844">
@@ -12323,7 +12323,7 @@
         <v>0.51</v>
       </c>
       <c r="C844" t="n">
-        <v>0.4166666666666667</v>
+        <v>0.4583333333333333</v>
       </c>
     </row>
     <row r="845">
@@ -12349,7 +12349,7 @@
         <v>0.53</v>
       </c>
       <c r="C846" t="n">
-        <v>0.4583333333333333</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="847">
@@ -12362,7 +12362,7 @@
         <v>0.54</v>
       </c>
       <c r="C847" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.7083333333333334</v>
       </c>
     </row>
     <row r="848">
@@ -12375,7 +12375,7 @@
         <v>0.55</v>
       </c>
       <c r="C848" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.9166666666666666</v>
       </c>
     </row>
     <row r="849">
@@ -12427,7 +12427,7 @@
         <v>0.59</v>
       </c>
       <c r="C852" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.9583333333333334</v>
       </c>
     </row>
     <row r="853">
@@ -12440,7 +12440,7 @@
         <v>0.6</v>
       </c>
       <c r="C853" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.9583333333333334</v>
       </c>
     </row>
     <row r="854">
@@ -12453,7 +12453,7 @@
         <v>0.61</v>
       </c>
       <c r="C854" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.9583333333333334</v>
       </c>
     </row>
     <row r="855">
@@ -12466,7 +12466,7 @@
         <v>0.62</v>
       </c>
       <c r="C855" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.9583333333333334</v>
       </c>
     </row>
     <row r="856">
@@ -12479,7 +12479,7 @@
         <v>0.63</v>
       </c>
       <c r="C856" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.9583333333333334</v>
       </c>
     </row>
     <row r="857">
@@ -12492,7 +12492,7 @@
         <v>0.64</v>
       </c>
       <c r="C857" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.9583333333333334</v>
       </c>
     </row>
     <row r="858">
@@ -12505,7 +12505,7 @@
         <v>0.65</v>
       </c>
       <c r="C858" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.9583333333333334</v>
       </c>
     </row>
     <row r="859">
@@ -12518,7 +12518,7 @@
         <v>0.66</v>
       </c>
       <c r="C859" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.9583333333333334</v>
       </c>
     </row>
     <row r="860">
@@ -12531,7 +12531,7 @@
         <v>0.67</v>
       </c>
       <c r="C860" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.9583333333333334</v>
       </c>
     </row>
     <row r="861">
@@ -12908,7 +12908,7 @@
         <v>0.9600000000000001</v>
       </c>
       <c r="C889" t="n">
-        <v>0.9583333333333334</v>
+        <v>1</v>
       </c>
     </row>
     <row r="890">
@@ -12921,7 +12921,7 @@
         <v>0.97</v>
       </c>
       <c r="C890" t="n">
-        <v>0.9583333333333334</v>
+        <v>1</v>
       </c>
     </row>
     <row r="891">
@@ -12934,7 +12934,7 @@
         <v>0.98</v>
       </c>
       <c r="C891" t="n">
-        <v>0.9583333333333334</v>
+        <v>1</v>
       </c>
     </row>
     <row r="892">
@@ -12947,7 +12947,7 @@
         <v>0.99</v>
       </c>
       <c r="C892" t="n">
-        <v>0.9583333333333334</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cambios en los analisis
</commit_message>
<xml_diff>
--- a/codigo_final_organizado/Aplicaciones/Aplicaciones_puras/Resultados_Electricity_Final/electricity_serie_0_resultados_full.xlsx
+++ b/codigo_final_organizado/Aplicaciones/Aplicaciones_puras/Resultados_Electricity_Final/electricity_serie_0_resultados_full.xlsx
@@ -508,7 +508,7 @@
         <v>0.9089724895519442</v>
       </c>
       <c r="F2" t="n">
-        <v>0.742089424612141</v>
+        <v>1.094843486897785</v>
       </c>
       <c r="G2" t="n">
         <v>4.940678770078736</v>
@@ -523,7 +523,7 @@
         <v>2.925520793545424</v>
       </c>
       <c r="K2" t="n">
-        <v>2.032902704351438</v>
+        <v>1.931720668638357</v>
       </c>
     </row>
     <row r="3">
@@ -543,7 +543,7 @@
         <v>1.239889758575947</v>
       </c>
       <c r="F3" t="n">
-        <v>2.953359325571835</v>
+        <v>1.486570876490288</v>
       </c>
       <c r="G3" t="n">
         <v>1.212355103492718</v>
@@ -558,7 +558,7 @@
         <v>2.594210902604413</v>
       </c>
       <c r="K3" t="n">
-        <v>2.230793648659107</v>
+        <v>1.774554667157681</v>
       </c>
     </row>
     <row r="4">
@@ -578,7 +578,7 @@
         <v>3.473868903179205</v>
       </c>
       <c r="F4" t="n">
-        <v>3.777279631906095</v>
+        <v>3.619089232280891</v>
       </c>
       <c r="G4" t="n">
         <v>1.075063255536551</v>
@@ -593,7 +593,7 @@
         <v>1.960757881245542</v>
       </c>
       <c r="K4" t="n">
-        <v>1.93969075190823</v>
+        <v>1.60116207856829</v>
       </c>
     </row>
     <row r="5">
@@ -613,7 +613,7 @@
         <v>0.938654534349344</v>
       </c>
       <c r="F5" t="n">
-        <v>2.953359325571833</v>
+        <v>1.233928876218327</v>
       </c>
       <c r="G5" t="n">
         <v>1.210893091312481</v>
@@ -628,7 +628,7 @@
         <v>1.525057750975637</v>
       </c>
       <c r="K5" t="n">
-        <v>1.646847391502495</v>
+        <v>1.262763469482181</v>
       </c>
     </row>
     <row r="6">
@@ -648,7 +648,7 @@
         <v>0.7248606801997122</v>
       </c>
       <c r="F6" t="n">
-        <v>2.953359325571836</v>
+        <v>0.9823049001344488</v>
       </c>
       <c r="G6" t="n">
         <v>1.209984847847151</v>
@@ -663,7 +663,7 @@
         <v>1.52716259180392</v>
       </c>
       <c r="K6" t="n">
-        <v>1.668739007363945</v>
+        <v>1.279973487446525</v>
       </c>
     </row>
     <row r="7">
@@ -683,7 +683,7 @@
         <v>1.181586493633075</v>
       </c>
       <c r="F7" t="n">
-        <v>3.777279631906094</v>
+        <v>1.392601770540418</v>
       </c>
       <c r="G7" t="n">
         <v>1.074203496262546</v>
@@ -698,7 +698,7 @@
         <v>2.089103999035299</v>
       </c>
       <c r="K7" t="n">
-        <v>1.788909442203023</v>
+        <v>1.438220153790516</v>
       </c>
     </row>
     <row r="8">
@@ -718,7 +718,7 @@
         <v>0.7449034850928795</v>
       </c>
       <c r="F8" t="n">
-        <v>2.953359325571834</v>
+        <v>1.017997578999949</v>
       </c>
       <c r="G8" t="n">
         <v>1.208266822396189</v>
@@ -733,7 +733,7 @@
         <v>1.732208502183915</v>
       </c>
       <c r="K8" t="n">
-        <v>1.700551401900429</v>
+        <v>1.306575586663374</v>
       </c>
     </row>
     <row r="9">
@@ -753,7 +753,7 @@
         <v>0.7734660688444341</v>
       </c>
       <c r="F9" t="n">
-        <v>2.953359325571834</v>
+        <v>0.9193417331874425</v>
       </c>
       <c r="G9" t="n">
         <v>1.207495796356991</v>
@@ -768,7 +768,7 @@
         <v>1.781945169349529</v>
       </c>
       <c r="K9" t="n">
-        <v>1.691681735588474</v>
+        <v>1.303238997068369</v>
       </c>
     </row>
     <row r="10">
@@ -788,7 +788,7 @@
         <v>0.7296248096678344</v>
       </c>
       <c r="F10" t="n">
-        <v>2.953359325571833</v>
+        <v>0.9228100604296587</v>
       </c>
       <c r="G10" t="n">
         <v>1.206807832719729</v>
@@ -803,7 +803,7 @@
         <v>1.643567142013495</v>
       </c>
       <c r="K10" t="n">
-        <v>1.6870531869567</v>
+        <v>1.303522739277548</v>
       </c>
     </row>
     <row r="11">
@@ -823,7 +823,7 @@
         <v>0.929847020305707</v>
       </c>
       <c r="F11" t="n">
-        <v>3.777279631906095</v>
+        <v>1.149347150335248</v>
       </c>
       <c r="G11" t="n">
         <v>1.073400461998491</v>
@@ -838,7 +838,7 @@
         <v>1.844681550063179</v>
       </c>
       <c r="K11" t="n">
-        <v>1.7749306112228</v>
+        <v>1.42523552514246</v>
       </c>
     </row>
     <row r="12">
@@ -858,7 +858,7 @@
         <v>1.29355712309134</v>
       </c>
       <c r="F12" t="n">
-        <v>1.401967866115882</v>
+        <v>1.250137702019458</v>
       </c>
       <c r="G12" t="n">
         <v>2.270147657429868</v>
@@ -873,7 +873,7 @@
         <v>1.715717939514911</v>
       </c>
       <c r="K12" t="n">
-        <v>1.950960876780078</v>
+        <v>1.601997735848329</v>
       </c>
     </row>
     <row r="13">
@@ -893,7 +893,7 @@
         <v>2.369194362372474</v>
       </c>
       <c r="F13" t="n">
-        <v>0.7999390277312268</v>
+        <v>2.34864136949764</v>
       </c>
       <c r="G13" t="n">
         <v>3.062716945528508</v>
@@ -908,7 +908,7 @@
         <v>1.33706758191068</v>
       </c>
       <c r="K13" t="n">
-        <v>1.819000407277076</v>
+        <v>1.499226493434675</v>
       </c>
     </row>
     <row r="14">
@@ -928,7 +928,7 @@
         <v>6.226984032392564</v>
       </c>
       <c r="F14" t="n">
-        <v>9.054895014197431</v>
+        <v>6.173114231876883</v>
       </c>
       <c r="G14" t="n">
         <v>3.905806203603865</v>
@@ -943,7 +943,7 @@
         <v>5.637124946295703</v>
       </c>
       <c r="K14" t="n">
-        <v>5.734071476362839</v>
+        <v>5.640417840643222</v>
       </c>
     </row>
     <row r="15">
@@ -963,7 +963,7 @@
         <v>23.1121475027579</v>
       </c>
       <c r="F15" t="n">
-        <v>25.99871894680209</v>
+        <v>22.65061988648479</v>
       </c>
       <c r="G15" t="n">
         <v>18.00929787837195</v>
@@ -978,7 +978,7 @@
         <v>13.74946082406465</v>
       </c>
       <c r="K15" t="n">
-        <v>18.00500237850628</v>
+        <v>18.27065360367348</v>
       </c>
     </row>
     <row r="16">
@@ -998,7 +998,7 @@
         <v>5.404099587475494</v>
       </c>
       <c r="F16" t="n">
-        <v>0.7999390277312264</v>
+        <v>5.356462118557237</v>
       </c>
       <c r="G16" t="n">
         <v>3.05419614748985</v>
@@ -1013,7 +1013,7 @@
         <v>9.895269065787287</v>
       </c>
       <c r="K16" t="n">
-        <v>8.375835186681101</v>
+        <v>12.27082204778578</v>
       </c>
     </row>
     <row r="17">
@@ -1033,7 +1033,7 @@
         <v>18.70977284719968</v>
       </c>
       <c r="F17" t="n">
-        <v>0.7420894246121428</v>
+        <v>18.09385031192362</v>
       </c>
       <c r="G17" t="n">
         <v>4.908726407000762</v>
@@ -1048,7 +1048,7 @@
         <v>1.6057583227182</v>
       </c>
       <c r="K17" t="n">
-        <v>3.263949372709502</v>
+        <v>3.665214953816475</v>
       </c>
     </row>
     <row r="18">
@@ -1068,7 +1068,7 @@
         <v>4.071656435147918</v>
       </c>
       <c r="F18" t="n">
-        <v>0.7420894246121423</v>
+        <v>3.902683327859297</v>
       </c>
       <c r="G18" t="n">
         <v>4.906448829503312</v>
@@ -1083,7 +1083,7 @@
         <v>2.45521316539933</v>
       </c>
       <c r="K18" t="n">
-        <v>2.375325059849129</v>
+        <v>2.165901822506475</v>
       </c>
     </row>
     <row r="19">
@@ -1103,7 +1103,7 @@
         <v>3.437504934532319</v>
       </c>
       <c r="F19" t="n">
-        <v>1.924183610532008</v>
+        <v>3.264356045331446</v>
       </c>
       <c r="G19" t="n">
         <v>6.867104908099141</v>
@@ -1118,7 +1118,7 @@
         <v>3.211364490559203</v>
       </c>
       <c r="K19" t="n">
-        <v>2.675805090820443</v>
+        <v>3.143172942916446</v>
       </c>
     </row>
     <row r="20">
@@ -1138,7 +1138,7 @@
         <v>3.15390497787076</v>
       </c>
       <c r="F20" t="n">
-        <v>1.924183610532008</v>
+        <v>2.939759479724035</v>
       </c>
       <c r="G20" t="n">
         <v>6.864224774588729</v>
@@ -1153,7 +1153,7 @@
         <v>2.660586763748931</v>
       </c>
       <c r="K20" t="n">
-        <v>2.936485144773834</v>
+        <v>2.512401568977887</v>
       </c>
     </row>
     <row r="21">
@@ -1173,7 +1173,7 @@
         <v>0.901219436440404</v>
       </c>
       <c r="F21" t="n">
-        <v>0.7420894246121419</v>
+        <v>1.034162089900195</v>
       </c>
       <c r="G21" t="n">
         <v>4.899832795597596</v>
@@ -1188,7 +1188,7 @@
         <v>2.183669486298967</v>
       </c>
       <c r="K21" t="n">
-        <v>1.869076177355903</v>
+        <v>1.169697342286949</v>
       </c>
     </row>
     <row r="22">
@@ -1208,7 +1208,7 @@
         <v>3.096962819698118</v>
       </c>
       <c r="F22" t="n">
-        <v>2.147422685988766</v>
+        <v>3.146106440486252</v>
       </c>
       <c r="G22" t="n">
         <v>1.616030202044811</v>
@@ -1223,7 +1223,7 @@
         <v>1.374940234592161</v>
       </c>
       <c r="K22" t="n">
-        <v>1.395298584892969</v>
+        <v>1.565641890606473</v>
       </c>
     </row>
     <row r="23">
@@ -1243,7 +1243,7 @@
         <v>1.700602675297426</v>
       </c>
       <c r="F23" t="n">
-        <v>0.7999390277312268</v>
+        <v>1.813293355726139</v>
       </c>
       <c r="G23" t="n">
         <v>3.040700413117551</v>
@@ -1258,7 +1258,7 @@
         <v>2.029910122480708</v>
       </c>
       <c r="K23" t="n">
-        <v>1.425312474453537</v>
+        <v>1.149813814785394</v>
       </c>
     </row>
     <row r="24">
@@ -1278,7 +1278,7 @@
         <v>1.822802768202143</v>
       </c>
       <c r="F24" t="n">
-        <v>2.953359325571834</v>
+        <v>1.983541408887818</v>
       </c>
       <c r="G24" t="n">
         <v>1.199475397109882</v>
@@ -1293,7 +1293,7 @@
         <v>2.448133529151313</v>
       </c>
       <c r="K24" t="n">
-        <v>1.988700028216392</v>
+        <v>1.605174468710672</v>
       </c>
     </row>
     <row r="25">
@@ -1313,7 +1313,7 @@
         <v>1.037410490359387</v>
       </c>
       <c r="F25" t="n">
-        <v>1.40196786611588</v>
+        <v>1.255810196405068</v>
       </c>
       <c r="G25" t="n">
         <v>2.248012146681598</v>
@@ -1328,7 +1328,7 @@
         <v>1.442606730237687</v>
       </c>
       <c r="K25" t="n">
-        <v>1.508925258103195</v>
+        <v>1.173978629027736</v>
       </c>
     </row>
   </sheetData>
@@ -5277,7 +5277,7 @@
         <v>0.04</v>
       </c>
       <c r="C302" t="n">
-        <v>0</v>
+        <v>0.04166666666666666</v>
       </c>
     </row>
     <row r="303">
@@ -5290,7 +5290,7 @@
         <v>0.05</v>
       </c>
       <c r="C303" t="n">
-        <v>0</v>
+        <v>0.04166666666666666</v>
       </c>
     </row>
     <row r="304">
@@ -5303,7 +5303,7 @@
         <v>0.06</v>
       </c>
       <c r="C304" t="n">
-        <v>0</v>
+        <v>0.04166666666666666</v>
       </c>
     </row>
     <row r="305">
@@ -5316,7 +5316,7 @@
         <v>0.06999999999999999</v>
       </c>
       <c r="C305" t="n">
-        <v>0</v>
+        <v>0.08333333333333333</v>
       </c>
     </row>
     <row r="306">
@@ -5329,7 +5329,7 @@
         <v>0.08</v>
       </c>
       <c r="C306" t="n">
-        <v>0</v>
+        <v>0.08333333333333333</v>
       </c>
     </row>
     <row r="307">
@@ -5342,7 +5342,7 @@
         <v>0.09</v>
       </c>
       <c r="C307" t="n">
-        <v>0</v>
+        <v>0.08333333333333333</v>
       </c>
     </row>
     <row r="308">
@@ -5355,7 +5355,7 @@
         <v>0.09999999999999999</v>
       </c>
       <c r="C308" t="n">
-        <v>0</v>
+        <v>0.08333333333333333</v>
       </c>
     </row>
     <row r="309">
@@ -5368,7 +5368,7 @@
         <v>0.11</v>
       </c>
       <c r="C309" t="n">
-        <v>0</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="310">
@@ -5381,7 +5381,7 @@
         <v>0.12</v>
       </c>
       <c r="C310" t="n">
-        <v>0</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="311">
@@ -5394,7 +5394,7 @@
         <v>0.13</v>
       </c>
       <c r="C311" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="312">
@@ -5407,7 +5407,7 @@
         <v>0.14</v>
       </c>
       <c r="C312" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="313">
@@ -5420,7 +5420,7 @@
         <v>0.15</v>
       </c>
       <c r="C313" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.2083333333333333</v>
       </c>
     </row>
     <row r="314">
@@ -5433,7 +5433,7 @@
         <v>0.16</v>
       </c>
       <c r="C314" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="315">
@@ -5446,7 +5446,7 @@
         <v>0.17</v>
       </c>
       <c r="C315" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="316">
@@ -5459,7 +5459,7 @@
         <v>0.18</v>
       </c>
       <c r="C316" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="317">
@@ -5472,7 +5472,7 @@
         <v>0.19</v>
       </c>
       <c r="C317" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="318">
@@ -5485,7 +5485,7 @@
         <v>0.2</v>
       </c>
       <c r="C318" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="319">
@@ -5498,7 +5498,7 @@
         <v>0.21</v>
       </c>
       <c r="C319" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="320">
@@ -5511,7 +5511,7 @@
         <v>0.22</v>
       </c>
       <c r="C320" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="321">
@@ -5524,7 +5524,7 @@
         <v>0.23</v>
       </c>
       <c r="C321" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="322">
@@ -5537,7 +5537,7 @@
         <v>0.24</v>
       </c>
       <c r="C322" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="323">
@@ -5550,7 +5550,7 @@
         <v>0.25</v>
       </c>
       <c r="C323" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="324">
@@ -5563,7 +5563,7 @@
         <v>0.26</v>
       </c>
       <c r="C324" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="325">
@@ -5576,7 +5576,7 @@
         <v>0.27</v>
       </c>
       <c r="C325" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.2916666666666667</v>
       </c>
     </row>
     <row r="326">
@@ -5589,7 +5589,7 @@
         <v>0.28</v>
       </c>
       <c r="C326" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.2916666666666667</v>
       </c>
     </row>
     <row r="327">
@@ -5602,7 +5602,7 @@
         <v>0.29</v>
       </c>
       <c r="C327" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.2916666666666667</v>
       </c>
     </row>
     <row r="328">
@@ -5615,7 +5615,7 @@
         <v>0.3</v>
       </c>
       <c r="C328" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.2916666666666667</v>
       </c>
     </row>
     <row r="329">
@@ -5628,7 +5628,7 @@
         <v>0.31</v>
       </c>
       <c r="C329" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.2916666666666667</v>
       </c>
     </row>
     <row r="330">
@@ -5641,7 +5641,7 @@
         <v>0.32</v>
       </c>
       <c r="C330" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.2916666666666667</v>
       </c>
     </row>
     <row r="331">
@@ -5654,7 +5654,7 @@
         <v>0.33</v>
       </c>
       <c r="C331" t="n">
-        <v>0.25</v>
+        <v>0.2916666666666667</v>
       </c>
     </row>
     <row r="332">
@@ -5667,7 +5667,7 @@
         <v>0.34</v>
       </c>
       <c r="C332" t="n">
-        <v>0.25</v>
+        <v>0.2916666666666667</v>
       </c>
     </row>
     <row r="333">
@@ -5680,7 +5680,7 @@
         <v>0.35</v>
       </c>
       <c r="C333" t="n">
-        <v>0.25</v>
+        <v>0.2916666666666667</v>
       </c>
     </row>
     <row r="334">
@@ -5693,7 +5693,7 @@
         <v>0.36</v>
       </c>
       <c r="C334" t="n">
-        <v>0.25</v>
+        <v>0.2916666666666667</v>
       </c>
     </row>
     <row r="335">
@@ -5706,7 +5706,7 @@
         <v>0.37</v>
       </c>
       <c r="C335" t="n">
-        <v>0.25</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="336">
@@ -5719,7 +5719,7 @@
         <v>0.38</v>
       </c>
       <c r="C336" t="n">
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="337">
@@ -5732,7 +5732,7 @@
         <v>0.39</v>
       </c>
       <c r="C337" t="n">
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="338">
@@ -5745,7 +5745,7 @@
         <v>0.4</v>
       </c>
       <c r="C338" t="n">
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="339">
@@ -5758,7 +5758,7 @@
         <v>0.41</v>
       </c>
       <c r="C339" t="n">
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="340">
@@ -5771,7 +5771,7 @@
         <v>0.42</v>
       </c>
       <c r="C340" t="n">
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="341">
@@ -5784,7 +5784,7 @@
         <v>0.43</v>
       </c>
       <c r="C341" t="n">
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="342">
@@ -5797,7 +5797,7 @@
         <v>0.44</v>
       </c>
       <c r="C342" t="n">
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="343">
@@ -5810,7 +5810,7 @@
         <v>0.45</v>
       </c>
       <c r="C343" t="n">
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="344">
@@ -5823,7 +5823,7 @@
         <v>0.46</v>
       </c>
       <c r="C344" t="n">
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="345">
@@ -5836,7 +5836,7 @@
         <v>0.47</v>
       </c>
       <c r="C345" t="n">
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="346">
@@ -5849,7 +5849,7 @@
         <v>0.48</v>
       </c>
       <c r="C346" t="n">
-        <v>0.25</v>
+        <v>0.4166666666666667</v>
       </c>
     </row>
     <row r="347">
@@ -5862,7 +5862,7 @@
         <v>0.49</v>
       </c>
       <c r="C347" t="n">
-        <v>0.25</v>
+        <v>0.4583333333333333</v>
       </c>
     </row>
     <row r="348">
@@ -5875,7 +5875,7 @@
         <v>0.5</v>
       </c>
       <c r="C348" t="n">
-        <v>0.25</v>
+        <v>0.4583333333333333</v>
       </c>
     </row>
     <row r="349">
@@ -5888,7 +5888,7 @@
         <v>0.51</v>
       </c>
       <c r="C349" t="n">
-        <v>0.25</v>
+        <v>0.4583333333333333</v>
       </c>
     </row>
     <row r="350">
@@ -5901,7 +5901,7 @@
         <v>0.52</v>
       </c>
       <c r="C350" t="n">
-        <v>0.25</v>
+        <v>0.4583333333333333</v>
       </c>
     </row>
     <row r="351">
@@ -5914,7 +5914,7 @@
         <v>0.53</v>
       </c>
       <c r="C351" t="n">
-        <v>0.25</v>
+        <v>0.4583333333333333</v>
       </c>
     </row>
     <row r="352">
@@ -5927,7 +5927,7 @@
         <v>0.54</v>
       </c>
       <c r="C352" t="n">
-        <v>0.25</v>
+        <v>0.4583333333333333</v>
       </c>
     </row>
     <row r="353">
@@ -5940,7 +5940,7 @@
         <v>0.55</v>
       </c>
       <c r="C353" t="n">
-        <v>0.25</v>
+        <v>0.4583333333333333</v>
       </c>
     </row>
     <row r="354">
@@ -5953,7 +5953,7 @@
         <v>0.5600000000000001</v>
       </c>
       <c r="C354" t="n">
-        <v>0.25</v>
+        <v>0.4583333333333333</v>
       </c>
     </row>
     <row r="355">
@@ -5966,7 +5966,7 @@
         <v>0.5700000000000001</v>
       </c>
       <c r="C355" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="356">
@@ -5979,7 +5979,7 @@
         <v>0.5800000000000001</v>
       </c>
       <c r="C356" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="357">
@@ -5992,7 +5992,7 @@
         <v>0.59</v>
       </c>
       <c r="C357" t="n">
-        <v>0.25</v>
+        <v>0.5416666666666666</v>
       </c>
     </row>
     <row r="358">
@@ -6005,7 +6005,7 @@
         <v>0.6</v>
       </c>
       <c r="C358" t="n">
-        <v>0.25</v>
+        <v>0.5416666666666666</v>
       </c>
     </row>
     <row r="359">
@@ -6018,7 +6018,7 @@
         <v>0.61</v>
       </c>
       <c r="C359" t="n">
-        <v>0.25</v>
+        <v>0.5416666666666666</v>
       </c>
     </row>
     <row r="360">
@@ -6031,7 +6031,7 @@
         <v>0.62</v>
       </c>
       <c r="C360" t="n">
-        <v>0.25</v>
+        <v>0.5416666666666666</v>
       </c>
     </row>
     <row r="361">
@@ -6044,7 +6044,7 @@
         <v>0.63</v>
       </c>
       <c r="C361" t="n">
-        <v>0.25</v>
+        <v>0.5416666666666666</v>
       </c>
     </row>
     <row r="362">
@@ -6057,7 +6057,7 @@
         <v>0.64</v>
       </c>
       <c r="C362" t="n">
-        <v>0.25</v>
+        <v>0.5416666666666666</v>
       </c>
     </row>
     <row r="363">
@@ -6070,7 +6070,7 @@
         <v>0.65</v>
       </c>
       <c r="C363" t="n">
-        <v>0.25</v>
+        <v>0.5416666666666666</v>
       </c>
     </row>
     <row r="364">
@@ -6083,7 +6083,7 @@
         <v>0.66</v>
       </c>
       <c r="C364" t="n">
-        <v>0.25</v>
+        <v>0.5416666666666666</v>
       </c>
     </row>
     <row r="365">
@@ -6096,7 +6096,7 @@
         <v>0.67</v>
       </c>
       <c r="C365" t="n">
-        <v>0.25</v>
+        <v>0.5833333333333334</v>
       </c>
     </row>
     <row r="366">
@@ -6109,7 +6109,7 @@
         <v>0.68</v>
       </c>
       <c r="C366" t="n">
-        <v>0.25</v>
+        <v>0.5833333333333334</v>
       </c>
     </row>
     <row r="367">
@@ -6122,7 +6122,7 @@
         <v>0.6900000000000001</v>
       </c>
       <c r="C367" t="n">
-        <v>0.25</v>
+        <v>0.5833333333333334</v>
       </c>
     </row>
     <row r="368">
@@ -6135,7 +6135,7 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="C368" t="n">
-        <v>0.25</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="369">
@@ -6148,7 +6148,7 @@
         <v>0.7100000000000001</v>
       </c>
       <c r="C369" t="n">
-        <v>0.25</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="370">
@@ -6161,7 +6161,7 @@
         <v>0.72</v>
       </c>
       <c r="C370" t="n">
-        <v>0.25</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="371">
@@ -6174,7 +6174,7 @@
         <v>0.73</v>
       </c>
       <c r="C371" t="n">
-        <v>0.25</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="372">
@@ -6187,7 +6187,7 @@
         <v>0.74</v>
       </c>
       <c r="C372" t="n">
-        <v>0.25</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="373">
@@ -6200,7 +6200,7 @@
         <v>0.75</v>
       </c>
       <c r="C373" t="n">
-        <v>0.375</v>
+        <v>0.7083333333333334</v>
       </c>
     </row>
     <row r="374">
@@ -6213,7 +6213,7 @@
         <v>0.76</v>
       </c>
       <c r="C374" t="n">
-        <v>0.375</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="375">
@@ -6226,7 +6226,7 @@
         <v>0.77</v>
       </c>
       <c r="C375" t="n">
-        <v>0.375</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="376">
@@ -6239,7 +6239,7 @@
         <v>0.78</v>
       </c>
       <c r="C376" t="n">
-        <v>0.375</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="377">
@@ -6252,7 +6252,7 @@
         <v>0.79</v>
       </c>
       <c r="C377" t="n">
-        <v>0.375</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="378">
@@ -6265,7 +6265,7 @@
         <v>0.8</v>
       </c>
       <c r="C378" t="n">
-        <v>0.375</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="379">
@@ -6278,7 +6278,7 @@
         <v>0.8100000000000001</v>
       </c>
       <c r="C379" t="n">
-        <v>0.375</v>
+        <v>0.8333333333333334</v>
       </c>
     </row>
     <row r="380">
@@ -6291,7 +6291,7 @@
         <v>0.8200000000000001</v>
       </c>
       <c r="C380" t="n">
-        <v>0.375</v>
+        <v>0.8333333333333334</v>
       </c>
     </row>
     <row r="381">
@@ -6304,7 +6304,7 @@
         <v>0.8300000000000001</v>
       </c>
       <c r="C381" t="n">
-        <v>0.375</v>
+        <v>0.8333333333333334</v>
       </c>
     </row>
     <row r="382">
@@ -6317,7 +6317,7 @@
         <v>0.8400000000000001</v>
       </c>
       <c r="C382" t="n">
-        <v>0.375</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="383">
@@ -6330,7 +6330,7 @@
         <v>0.85</v>
       </c>
       <c r="C383" t="n">
-        <v>0.4583333333333333</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="384">
@@ -6343,7 +6343,7 @@
         <v>0.86</v>
       </c>
       <c r="C384" t="n">
-        <v>0.4583333333333333</v>
+        <v>0.9166666666666666</v>
       </c>
     </row>
     <row r="385">
@@ -6356,7 +6356,7 @@
         <v>0.87</v>
       </c>
       <c r="C385" t="n">
-        <v>0.4583333333333333</v>
+        <v>0.9166666666666666</v>
       </c>
     </row>
     <row r="386">
@@ -6369,7 +6369,7 @@
         <v>0.88</v>
       </c>
       <c r="C386" t="n">
-        <v>0.4583333333333333</v>
+        <v>0.9166666666666666</v>
       </c>
     </row>
     <row r="387">
@@ -6382,7 +6382,7 @@
         <v>0.89</v>
       </c>
       <c r="C387" t="n">
-        <v>0.4583333333333333</v>
+        <v>0.9166666666666666</v>
       </c>
     </row>
     <row r="388">
@@ -6395,7 +6395,7 @@
         <v>0.9</v>
       </c>
       <c r="C388" t="n">
-        <v>0.5</v>
+        <v>0.9583333333333334</v>
       </c>
     </row>
     <row r="389">
@@ -6408,7 +6408,7 @@
         <v>0.91</v>
       </c>
       <c r="C389" t="n">
-        <v>0.7916666666666666</v>
+        <v>0.9583333333333334</v>
       </c>
     </row>
     <row r="390">
@@ -6421,7 +6421,7 @@
         <v>0.92</v>
       </c>
       <c r="C390" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.9583333333333334</v>
       </c>
     </row>
     <row r="391">
@@ -6434,7 +6434,7 @@
         <v>0.93</v>
       </c>
       <c r="C391" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.9583333333333334</v>
       </c>
     </row>
     <row r="392">
@@ -6447,7 +6447,7 @@
         <v>0.9400000000000001</v>
       </c>
       <c r="C392" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.9583333333333334</v>
       </c>
     </row>
     <row r="393">
@@ -6460,7 +6460,7 @@
         <v>0.9500000000000001</v>
       </c>
       <c r="C393" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.9583333333333334</v>
       </c>
     </row>
     <row r="394">
@@ -6473,7 +6473,7 @@
         <v>0.9600000000000001</v>
       </c>
       <c r="C394" t="n">
-        <v>0.9583333333333334</v>
+        <v>1</v>
       </c>
     </row>
     <row r="395">
@@ -6486,7 +6486,7 @@
         <v>0.97</v>
       </c>
       <c r="C395" t="n">
-        <v>0.9583333333333334</v>
+        <v>1</v>
       </c>
     </row>
     <row r="396">
@@ -6499,7 +6499,7 @@
         <v>0.98</v>
       </c>
       <c r="C396" t="n">
-        <v>0.9583333333333334</v>
+        <v>1</v>
       </c>
     </row>
     <row r="397">
@@ -11712,7 +11712,7 @@
         <v>0.04</v>
       </c>
       <c r="C797" t="n">
-        <v>0</v>
+        <v>0.04166666666666666</v>
       </c>
     </row>
     <row r="798">
@@ -11725,7 +11725,7 @@
         <v>0.05</v>
       </c>
       <c r="C798" t="n">
-        <v>0</v>
+        <v>0.04166666666666666</v>
       </c>
     </row>
     <row r="799">
@@ -11816,7 +11816,7 @@
         <v>0.12</v>
       </c>
       <c r="C805" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.08333333333333333</v>
       </c>
     </row>
     <row r="806">
@@ -11829,7 +11829,7 @@
         <v>0.13</v>
       </c>
       <c r="C806" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.08333333333333333</v>
       </c>
     </row>
     <row r="807">
@@ -11842,7 +11842,7 @@
         <v>0.14</v>
       </c>
       <c r="C807" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="808">
@@ -11855,7 +11855,7 @@
         <v>0.15</v>
       </c>
       <c r="C808" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="809">
@@ -11868,7 +11868,7 @@
         <v>0.16</v>
       </c>
       <c r="C809" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="810">
@@ -11881,7 +11881,7 @@
         <v>0.17</v>
       </c>
       <c r="C810" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="811">
@@ -11894,7 +11894,7 @@
         <v>0.18</v>
       </c>
       <c r="C811" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="812">
@@ -11907,7 +11907,7 @@
         <v>0.19</v>
       </c>
       <c r="C812" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="813">
@@ -11920,7 +11920,7 @@
         <v>0.2</v>
       </c>
       <c r="C813" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="814">
@@ -11933,7 +11933,7 @@
         <v>0.21</v>
       </c>
       <c r="C814" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="815">
@@ -11946,7 +11946,7 @@
         <v>0.22</v>
       </c>
       <c r="C815" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="816">
@@ -11959,7 +11959,7 @@
         <v>0.23</v>
       </c>
       <c r="C816" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="817">
@@ -11972,7 +11972,7 @@
         <v>0.24</v>
       </c>
       <c r="C817" t="n">
-        <v>0.125</v>
+        <v>0.2083333333333333</v>
       </c>
     </row>
     <row r="818">
@@ -11985,7 +11985,7 @@
         <v>0.25</v>
       </c>
       <c r="C818" t="n">
-        <v>0.125</v>
+        <v>0.2083333333333333</v>
       </c>
     </row>
     <row r="819">
@@ -11998,7 +11998,7 @@
         <v>0.26</v>
       </c>
       <c r="C819" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="820">
@@ -12011,7 +12011,7 @@
         <v>0.27</v>
       </c>
       <c r="C820" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="821">
@@ -12024,7 +12024,7 @@
         <v>0.28</v>
       </c>
       <c r="C821" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="822">
@@ -12037,7 +12037,7 @@
         <v>0.29</v>
       </c>
       <c r="C822" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="823">
@@ -12050,7 +12050,7 @@
         <v>0.3</v>
       </c>
       <c r="C823" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="824">
@@ -12063,7 +12063,7 @@
         <v>0.31</v>
       </c>
       <c r="C824" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="825">
@@ -12076,7 +12076,7 @@
         <v>0.32</v>
       </c>
       <c r="C825" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="826">
@@ -12089,7 +12089,7 @@
         <v>0.33</v>
       </c>
       <c r="C826" t="n">
-        <v>0.2916666666666667</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="827">
@@ -12102,7 +12102,7 @@
         <v>0.34</v>
       </c>
       <c r="C827" t="n">
-        <v>0.2916666666666667</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="828">
@@ -12128,7 +12128,7 @@
         <v>0.36</v>
       </c>
       <c r="C829" t="n">
-        <v>0.2916666666666667</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="830">
@@ -12141,7 +12141,7 @@
         <v>0.37</v>
       </c>
       <c r="C830" t="n">
-        <v>0.2916666666666667</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="831">
@@ -12154,7 +12154,7 @@
         <v>0.38</v>
       </c>
       <c r="C831" t="n">
-        <v>0.2916666666666667</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="832">
@@ -12167,7 +12167,7 @@
         <v>0.39</v>
       </c>
       <c r="C832" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="833">
@@ -12232,7 +12232,7 @@
         <v>0.44</v>
       </c>
       <c r="C837" t="n">
-        <v>0.375</v>
+        <v>0.4166666666666667</v>
       </c>
     </row>
     <row r="838">
@@ -12245,7 +12245,7 @@
         <v>0.45</v>
       </c>
       <c r="C838" t="n">
-        <v>0.375</v>
+        <v>0.4166666666666667</v>
       </c>
     </row>
     <row r="839">
@@ -12258,7 +12258,7 @@
         <v>0.46</v>
       </c>
       <c r="C839" t="n">
-        <v>0.375</v>
+        <v>0.4583333333333333</v>
       </c>
     </row>
     <row r="840">
@@ -12271,7 +12271,7 @@
         <v>0.47</v>
       </c>
       <c r="C840" t="n">
-        <v>0.375</v>
+        <v>0.4583333333333333</v>
       </c>
     </row>
     <row r="841">
@@ -12310,7 +12310,7 @@
         <v>0.5</v>
       </c>
       <c r="C843" t="n">
-        <v>0.5</v>
+        <v>0.4583333333333333</v>
       </c>
     </row>
     <row r="844">
@@ -12336,7 +12336,7 @@
         <v>0.52</v>
       </c>
       <c r="C845" t="n">
-        <v>0.5833333333333334</v>
+        <v>0.5416666666666666</v>
       </c>
     </row>
     <row r="846">
@@ -12362,7 +12362,7 @@
         <v>0.54</v>
       </c>
       <c r="C847" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="848">
@@ -12388,7 +12388,7 @@
         <v>0.5600000000000001</v>
       </c>
       <c r="C849" t="n">
-        <v>0.7083333333333334</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="850">
@@ -12401,7 +12401,7 @@
         <v>0.5700000000000001</v>
       </c>
       <c r="C850" t="n">
-        <v>0.7083333333333334</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="851">
@@ -12414,7 +12414,7 @@
         <v>0.5800000000000001</v>
       </c>
       <c r="C851" t="n">
-        <v>0.75</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="852">
@@ -12427,7 +12427,7 @@
         <v>0.59</v>
       </c>
       <c r="C852" t="n">
-        <v>0.7916666666666666</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="853">
@@ -12440,7 +12440,7 @@
         <v>0.6</v>
       </c>
       <c r="C853" t="n">
-        <v>0.7916666666666666</v>
+        <v>0.7083333333333334</v>
       </c>
     </row>
     <row r="854">
@@ -12453,7 +12453,7 @@
         <v>0.61</v>
       </c>
       <c r="C854" t="n">
-        <v>0.7916666666666666</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="855">
@@ -12466,7 +12466,7 @@
         <v>0.62</v>
       </c>
       <c r="C855" t="n">
-        <v>0.7916666666666666</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="856">
@@ -12479,7 +12479,7 @@
         <v>0.63</v>
       </c>
       <c r="C856" t="n">
-        <v>0.7916666666666666</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="857">
@@ -12492,7 +12492,7 @@
         <v>0.64</v>
       </c>
       <c r="C857" t="n">
-        <v>0.7916666666666666</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="858">
@@ -12505,7 +12505,7 @@
         <v>0.65</v>
       </c>
       <c r="C858" t="n">
-        <v>0.7916666666666666</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="859">
@@ -12518,7 +12518,7 @@
         <v>0.66</v>
       </c>
       <c r="C859" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="860">
@@ -12531,7 +12531,7 @@
         <v>0.67</v>
       </c>
       <c r="C860" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.7916666666666666</v>
       </c>
     </row>
     <row r="861">
@@ -12544,7 +12544,7 @@
         <v>0.68</v>
       </c>
       <c r="C861" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.7916666666666666</v>
       </c>
     </row>
     <row r="862">
@@ -12557,7 +12557,7 @@
         <v>0.6900000000000001</v>
       </c>
       <c r="C862" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.7916666666666666</v>
       </c>
     </row>
     <row r="863">
@@ -12570,7 +12570,7 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="C863" t="n">
-        <v>0.875</v>
+        <v>0.7916666666666666</v>
       </c>
     </row>
     <row r="864">
@@ -12596,7 +12596,7 @@
         <v>0.72</v>
       </c>
       <c r="C865" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="866">
@@ -12830,7 +12830,7 @@
         <v>0.9</v>
       </c>
       <c r="C883" t="n">
-        <v>0.9583333333333334</v>
+        <v>0.9166666666666666</v>
       </c>
     </row>
     <row r="884">
@@ -12843,7 +12843,7 @@
         <v>0.91</v>
       </c>
       <c r="C884" t="n">
-        <v>0.9583333333333334</v>
+        <v>0.9166666666666666</v>
       </c>
     </row>
     <row r="885">

</xml_diff>